<commit_message>
Developed a new test in catalog module - VerifyRequestor_changeRequire_ExistingLineLevel.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/UpdateCostCenter.xlsx
+++ b/src/test/resources/datasheets/UpdateCostCenter.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="15045" windowHeight="6210"/>
@@ -11,8 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -405,7 +404,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated Existing WorkBook with new input
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/UpdateCostCenter.xlsx
+++ b/src/test/resources/datasheets/UpdateCostCenter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15045" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15435" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="CostCenter" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Role</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>linelevel</t>
+  </si>
+  <si>
+    <t>QtyValue</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -106,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -414,7 +421,7 @@
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +452,11 @@
       <c r="J1" t="s">
         <v>12</v>
       </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -476,6 +486,9 @@
       </c>
       <c r="J2" t="s">
         <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Developed new Test "Verify_AddMoreItems", Updated WorkBook "UpdateCostCenter"
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/UpdateCostCenter.xlsx
+++ b/src/test/resources/datasheets/UpdateCostCenter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15045" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15435" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="CostCenter" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>Item Added Successfully</t>
   </si>
   <si>
-    <t>Computers</t>
-  </si>
-  <si>
     <t>EA-EACH</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>DeskTops</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -444,16 +444,16 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
       <c r="J1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -467,10 +467,10 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -479,16 +479,16 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Developed the following tests in catalog module: 1. Verify_BackButton_CartCheckConfirmRequest,and 2. Verify_ConfirmRequest_AddMoreItems.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/UpdateCostCenter.xlsx
+++ b/src/test/resources/datasheets/UpdateCostCenter.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="15435" windowHeight="6210"/>
@@ -11,8 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -412,11 +411,13 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E1" sqref="E1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="18.140625" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
   </cols>

</xml_diff>